<commit_message>
Power BOM now finished
All the BOMs done!
</commit_message>
<xml_diff>
--- a/BOM/powerBOM-RevA.xlsx
+++ b/BOM/powerBOM-RevA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t>TESA - Industrial Design Project - Summer 2014</t>
   </si>
@@ -55,19 +55,126 @@
   </si>
   <si>
     <t>Manufacturer PN</t>
+  </si>
+  <si>
+    <t>LED1,LED2,LED3</t>
+  </si>
+  <si>
+    <t>PLCC-4</t>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t>941-CLA1BWKWXD0F0DY3</t>
+  </si>
+  <si>
+    <t>Cree</t>
+  </si>
+  <si>
+    <t>CLA1B-WKW-XD0F0DY3</t>
+  </si>
+  <si>
+    <t>0.282/0.247/0.223</t>
+  </si>
+  <si>
+    <t>C101,C104</t>
+  </si>
+  <si>
+    <t>0.1u</t>
+  </si>
+  <si>
+    <t>SMD_0603</t>
+  </si>
+  <si>
+    <t>81-GRM39X104K16</t>
+  </si>
+  <si>
+    <t>Murata</t>
+  </si>
+  <si>
+    <t>GRM188R71C104KA01D</t>
+  </si>
+  <si>
+    <t>0.023/0.018/0.015</t>
+  </si>
+  <si>
+    <t>C401,C402</t>
+  </si>
+  <si>
+    <t>0.01u</t>
+  </si>
+  <si>
+    <t>81-GRM36X103K25</t>
+  </si>
+  <si>
+    <t>GRM155R71E103KA01D</t>
+  </si>
+  <si>
+    <t>0.117/0.014/0.008</t>
+  </si>
+  <si>
+    <t>TH hdr</t>
+  </si>
+  <si>
+    <t>653-XG8S-0231</t>
+  </si>
+  <si>
+    <t>Omron</t>
+  </si>
+  <si>
+    <t>XG8S-0231</t>
+  </si>
+  <si>
+    <t>for 25: 0.129/0.106/0.079</t>
+  </si>
+  <si>
+    <t>16 pins</t>
+  </si>
+  <si>
+    <t>3.3V</t>
+  </si>
+  <si>
+    <t>LD1117-TO-220</t>
+  </si>
+  <si>
+    <t>511-LD1117V33C</t>
+  </si>
+  <si>
+    <t>LD1117V33C</t>
+  </si>
+  <si>
+    <t>0.775/0.514/0.341</t>
+  </si>
+  <si>
+    <t>STMicroelectronics</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -87,13 +194,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -393,64 +509,288 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:I8"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="25.28515625" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" t="s">
+        <v>43</v>
+      </c>
+      <c r="I13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J13" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G11" r:id="rId1" tooltip="Click to view additional information on this product." display="http://ca.mouser.com/ProductDetail/Murata-Electronics/GRM155R71E103KA01D/?qs=sGAEpiMZZMsh%252b1woXyUXjw1hKv7JnOiP9oyPp5W%252bF4Y%3d"/>
+    <hyperlink ref="I11" r:id="rId2" display="http://ca.mouser.com/ProductDetail/Murata-Electronics/GRM155R71E103KA01D/?qs=sGAEpiMZZMsh%252b1woXyUXjw1hKv7JnOiP9oyPp5W%252bF4Y%3d"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>